<commit_message>
hour registration updated for myself and dirk
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation Verification and Validation\SVV-A10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3128A86-1C48-4D93-AB93-1C256C7916D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67D5B79-4EEB-499E-8342-273398AD5082}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Project group</t>
   </si>
@@ -60,31 +60,9 @@
     <t>week 3.3</t>
   </si>
   <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>xx</t>
-    </r>
-  </si>
-  <si>
     <t>student id</t>
   </si>
   <si>
-    <t>id1</t>
-  </si>
-  <si>
-    <t>id2</t>
-  </si>
-  <si>
     <t>id3</t>
   </si>
   <si>
@@ -95,6 +73,9 @@
   </si>
   <si>
     <t>id6</t>
+  </si>
+  <si>
+    <t>A10</t>
   </si>
 </sst>
 </file>
@@ -525,7 +506,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -548,25 +529,25 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11">
+        <v>4561619</v>
+      </c>
+      <c r="E4" s="11">
+        <v>4562771</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -576,34 +557,70 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -632,8 +649,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>4</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>

</xml_diff>

<commit_message>
Moved some stuff into the Modules folder to keep things organized
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\GitHub\SVV-A10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BC3609-9B73-4226-AB25-B191CE70445D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -241,7 +242,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,21 +519,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -540,7 +541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>13</v>
@@ -561,7 +562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -584,7 +585,7 @@
         <v>4532570</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -610,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -633,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -656,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -679,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -702,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -725,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -748,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -774,7 +775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -797,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>1</v>
       </c>
@@ -820,7 +821,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
@@ -831,7 +832,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>3</v>
       </c>
@@ -842,7 +843,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -853,7 +854,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>5</v>
       </c>
@@ -864,7 +865,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -878,7 +879,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -889,7 +890,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>1</v>
       </c>
@@ -900,7 +901,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>2</v>
       </c>
@@ -911,7 +912,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -922,7 +923,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -933,7 +934,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -944,7 +945,7 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
HourReg updated for Stijn and removed Data.txt from the main folder.
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BC3609-9B73-4226-AB25-B191CE70445D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D53219-5AD8-4900-B737-CF3DD5D43494}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +825,9 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -951,7 +953,7 @@
       </c>
       <c r="D29" s="12">
         <f>SUM(D5:D27)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E29" s="12">
         <f t="shared" ref="E29:I29" si="0">SUM(E5:E27)</f>

</xml_diff>

<commit_message>
changes to HourRegA10, Connected centroid and MOI to Main, coupled MOI and reaction forces
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BC3609-9B73-4226-AB25-B191CE70445D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -96,11 +93,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +117,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,7 +245,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -300,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -335,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -512,28 +515,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -541,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>13</v>
@@ -562,7 +565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -585,7 +588,7 @@
         <v>4532570</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -611,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -634,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -657,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -680,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -703,7 +706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -726,7 +729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -749,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -775,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -798,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9">
       <c r="C15" t="s">
         <v>1</v>
       </c>
@@ -821,18 +824,20 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9">
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6">
+        <v>3</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9">
       <c r="C17" t="s">
         <v>3</v>
       </c>
@@ -843,7 +848,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -854,7 +859,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9">
       <c r="C19" t="s">
         <v>5</v>
       </c>
@@ -865,7 +870,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -879,7 +884,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -890,7 +895,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9">
       <c r="C23" t="s">
         <v>1</v>
       </c>
@@ -901,7 +906,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9">
       <c r="C24" t="s">
         <v>2</v>
       </c>
@@ -912,7 +917,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9">
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -923,7 +928,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -934,7 +939,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -945,7 +950,7 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9">
       <c r="C29" t="s">
         <v>19</v>
       </c>
@@ -963,7 +968,7 @@
       </c>
       <c r="G29" s="12">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>27.5</v>
       </c>
       <c r="H29" s="12">
         <f t="shared" si="0"/>
@@ -975,7 +980,13 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All my changes of today's session
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D10D11-9C10-4520-895F-21B8DA25377D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045F8AAC-3497-4BCC-B19C-41E476A29FD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,14 +870,24 @@
       <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4</v>
+      </c>
       <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
@@ -982,19 +992,19 @@
       </c>
       <c r="D29" s="6">
         <f>SUM(D5:D27)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" ref="E29:I29" si="0">SUM(E5:E27)</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="0"/>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
@@ -1002,7 +1012,7 @@
       </c>
       <c r="I29" s="6">
         <f t="shared" si="0"/>
-        <v>28.25</v>
+        <v>32.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hour registration restored :)
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5136099-E11C-45D3-A145-B0BFEE081370}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -93,11 +96,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,12 +124,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,24 +225,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -303,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -338,7 +334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -515,28 +511,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>13</v>
@@ -565,7 +561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,7 +584,7 @@
         <v>4532570</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -637,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -660,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -683,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -706,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -729,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -752,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -778,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -801,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>1</v>
       </c>
@@ -820,57 +816,95 @@
       <c r="H15" s="6">
         <v>6.5</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="12">
         <v>5.75</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
       <c r="G16" s="6">
-        <v>3</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="2:9">
+        <v>2</v>
+      </c>
+      <c r="H16" s="6">
+        <v>5</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="F17" s="6">
+        <v>4</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8">
+        <v>1.5</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -881,10 +915,12 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -892,10 +928,12 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>1</v>
       </c>
@@ -906,7 +944,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>2</v>
       </c>
@@ -917,7 +955,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -928,7 +966,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -939,7 +977,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -950,43 +988,37 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="6">
         <f>SUM(D5:D27)</f>
-        <v>23</v>
-      </c>
-      <c r="E29" s="12">
+        <v>37.5</v>
+      </c>
+      <c r="E29" s="6">
         <f t="shared" ref="E29:I29" si="0">SUM(E5:E27)</f>
-        <v>21</v>
-      </c>
-      <c r="F29" s="12">
+        <v>29.5</v>
+      </c>
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G29" s="12">
+        <v>30</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="0"/>
+        <v>33.5</v>
+      </c>
+      <c r="H29" s="6">
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
-      <c r="H29" s="12">
+      <c r="I29" s="6">
         <f t="shared" si="0"/>
-        <v>22.5</v>
-      </c>
-      <c r="I29" s="12">
-        <f t="shared" si="0"/>
-        <v>23.75</v>
+        <v>32.25</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
saturday update hour registration
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="440" windowWidth="25600" windowHeight="14700"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,7 +519,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -915,7 +915,9 @@
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3">
+        <v>4</v>
+      </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
@@ -1007,7 +1009,7 @@
       </c>
       <c r="G29" s="6">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>43.5</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Hour reg update for all
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\GitHub\SVV-A10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotheken\Documenten\OneDrive\Stijn\Documenten\TU\3th Year\Simulation, Verification and Validation\SVV-A10\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AC503-9747-4D8D-A0A2-C6063A3D9174}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -243,7 +244,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,21 +521,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>13</v>
@@ -563,7 +564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -586,7 +587,7 @@
         <v>4532570</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -612,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -635,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -658,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -681,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -704,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -727,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -750,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -776,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -799,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>1</v>
       </c>
@@ -822,7 +823,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
@@ -845,7 +846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>3</v>
       </c>
@@ -868,7 +869,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -891,7 +892,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>5</v>
       </c>
@@ -912,7 +913,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -936,16 +937,20 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="5">
         <v>0.5</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
       <c r="H22" s="6">
         <v>0.5</v>
       </c>
@@ -953,33 +958,49 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="5">
         <v>5.5</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>5</v>
+      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="6">
+        <v>4.5</v>
+      </c>
       <c r="H23" s="6">
         <v>5</v>
       </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="7">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="5">
+        <v>4</v>
+      </c>
+      <c r="E24" s="6">
+        <v>4</v>
+      </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="6">
+        <v>4</v>
+      </c>
+      <c r="H24" s="6">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -990,7 +1011,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +1022,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -1012,17 +1033,17 @@
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="6">
         <f>SUM(D5:D27)</f>
-        <v>46.5</v>
+        <v>50.5</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" ref="E29:I29" si="0">SUM(E5:E27)</f>
-        <v>31.5</v>
+        <v>40.5</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
@@ -1030,15 +1051,15 @@
       </c>
       <c r="G29" s="6">
         <f t="shared" si="0"/>
-        <v>43.5</v>
+        <v>52</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="0"/>
-        <v>47.25</v>
+        <v>57.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validation data sorted for von mises stress
</commit_message>
<xml_diff>
--- a/HourRegistration_A10.xlsx
+++ b/HourRegistration_A10.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="B2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="6">
         <v>0.5</v>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E29" s="6">
         <f t="shared" ref="E29:I29" si="0">SUM(E5:E27)</f>
-        <v>45.5</v>
+        <v>46.5</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="J29" s="6">
         <f>AVERAGE(D29:I29)</f>
-        <v>50.625</v>
+        <v>50.791666666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>